<commit_message>
update dummy problem 2
</commit_message>
<xml_diff>
--- a/resources/problem01/Statistics.xlsx
+++ b/resources/problem01/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deb/github/WrittenQualifier/resources/problem01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588C62A0-3F2D-5D4F-A32C-D0E10BA8C12C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A693183-972D-8E4D-BF1D-4E693BC2F924}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28780" windowHeight="17540" xr2:uid="{977C3F12-CA30-2940-B949-BECFEB14FFE5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21500" windowHeight="17540" xr2:uid="{977C3F12-CA30-2940-B949-BECFEB14FFE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -250,6 +250,872 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$61:$H$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>467.56799999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1295.16336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1623.49896096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1877.8045204800001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2132.1100799999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2213.4669119999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-247F-C346-90C9-485CDF7F10B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2070164752"/>
+        <c:axId val="2064444976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2070164752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2064444976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2064444976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2070164752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>339182</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>22302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>760451</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>148063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4859CBBB-178F-0C4C-B348-27420CEFF7A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -549,17 +1415,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C57B4E5-0F7E-034B-88AC-01A388E6ED9A}">
-  <dimension ref="A2:S36"/>
+  <dimension ref="A2:S79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="82" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1252,6 +2122,209 @@
       </c>
       <c r="I36" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I51">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C52" s="4">
+        <v>144</v>
+      </c>
+      <c r="D52" s="4">
+        <v>398.88</v>
+      </c>
+      <c r="E52" s="4">
+        <v>499.99968000000001</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4">
+        <v>656.64</v>
+      </c>
+      <c r="H52" s="4">
+        <v>681.69600000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <f t="shared" ref="C53:G53" si="3">C52*10^6*$I$51</f>
+        <v>467568000000</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>1295163360000</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="3"/>
+        <v>1623498960960</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="3"/>
+        <v>2132110080000</v>
+      </c>
+      <c r="H53">
+        <f>H52*10^6*$I$51</f>
+        <v>2213466912000</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <f t="shared" ref="C54:G54" si="4">C53/(1000*1000*1000)</f>
+        <v>467.56799999999998</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="4"/>
+        <v>1295.16336</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="4"/>
+        <v>1623.49896096</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="4"/>
+        <v>2132.1100799999999</v>
+      </c>
+      <c r="H54">
+        <f>H53/(1000*1000*1000)</f>
+        <v>2213.4669119999999</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>2009</v>
+      </c>
+      <c r="C60">
+        <v>2013</v>
+      </c>
+      <c r="D60">
+        <v>2014</v>
+      </c>
+      <c r="E60">
+        <v>2015</v>
+      </c>
+      <c r="F60">
+        <v>2016</v>
+      </c>
+      <c r="G60">
+        <v>2017</v>
+      </c>
+      <c r="H60">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>467.56799999999998</v>
+      </c>
+      <c r="D61">
+        <v>1295.16336</v>
+      </c>
+      <c r="E61">
+        <v>1623.49896096</v>
+      </c>
+      <c r="F61">
+        <f>(E61+G61)/2</f>
+        <v>1877.8045204800001</v>
+      </c>
+      <c r="G61">
+        <v>2132.1100799999999</v>
+      </c>
+      <c r="H61">
+        <v>2213.4669119999999</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <f>(C61+B61)/2</f>
+        <v>283.78399999999999</v>
+      </c>
+      <c r="C63">
+        <f>(D61+C61)/2</f>
+        <v>881.36568</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ref="D63:G63" si="5">(E61+D61)/2</f>
+        <v>1459.3311604800001</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="5"/>
+        <v>1750.6517407199999</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="5"/>
+        <v>2004.95730024</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="5"/>
+        <v>2172.7884960000001</v>
+      </c>
+      <c r="H63">
+        <f>SUM(B63:G63)</f>
+        <v>8552.8783774399999</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <f>H63*365</f>
+        <v>3121800.6077656001</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C76" s="4">
+        <v>69120</v>
+      </c>
+      <c r="D76" s="4">
+        <v>103680</v>
+      </c>
+      <c r="E76" s="4">
+        <v>432000</v>
+      </c>
+      <c r="F76" s="4">
+        <v>576000</v>
+      </c>
+      <c r="G76" s="4">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C78">
+        <f>(D76+C76)/2</f>
+        <v>86400</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ref="D78:G78" si="6">(E76+D76)/2</f>
+        <v>267840</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="6"/>
+        <v>504000</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="6"/>
+        <v>648000</v>
+      </c>
+      <c r="H78">
+        <f>SUM(C78:F78)</f>
+        <v>1506240</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <f>60 * 93.8614355 * 365 *H78</f>
+        <v>3096174884504.688</v>
       </c>
     </row>
   </sheetData>
@@ -1264,5 +2337,6 @@
     <mergeCell ref="A24:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>